<commit_message>
:: to : in time
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2022.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5447" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="66">
   <si>
     <t>Waterpeil aanpassingen Veurne - Ambacht</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>1 x 0,40m</t>
-  </si>
-  <si>
-    <t>23::13</t>
   </si>
   <si>
     <t>1 x  0,20</t>
@@ -7718,8 +7715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L320"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10419,8 +10416,8 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="23"/>
-      <c r="B124" s="24" t="s">
-        <v>60</v>
+      <c r="B124" s="24">
+        <v>0.96736111111111101</v>
       </c>
       <c r="C124" s="25">
         <v>2.11</v>
@@ -10659,7 +10656,7 @@
         <v>10</v>
       </c>
       <c r="G134" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H134" s="32" t="s">
         <v>12</v>
@@ -10709,7 +10706,7 @@
         <v>10</v>
       </c>
       <c r="G136" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H136" s="32"/>
     </row>
@@ -10771,7 +10768,7 @@
         <v>10</v>
       </c>
       <c r="G139" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H139" s="32" t="s">
         <v>12</v>
@@ -10819,7 +10816,7 @@
         <v>10</v>
       </c>
       <c r="G141" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H141" s="32"/>
     </row>
@@ -16080,7 +16077,7 @@
         <v>10</v>
       </c>
       <c r="G74" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H74" s="32"/>
     </row>
@@ -16192,7 +16189,7 @@
         <v>10</v>
       </c>
       <c r="G79" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H79" s="32"/>
     </row>
@@ -16278,7 +16275,7 @@
         <v>10</v>
       </c>
       <c r="G83" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H83" s="32" t="s">
         <v>15</v>
@@ -16329,7 +16326,7 @@
         <v>14</v>
       </c>
       <c r="H85" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
@@ -17350,7 +17347,7 @@
         <v>10</v>
       </c>
       <c r="G131" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H131" s="32"/>
     </row>
@@ -26945,7 +26942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+    <sheetView topLeftCell="A265" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>

</xml_diff>